<commit_message>
Final changes and finished program
Uploading final changes to program. Executable file for final product made and stored separately and not in repo. Note main.exe and gasPrices.xlsx file must be stored in same folder for program to work and files must have those names.
</commit_message>
<xml_diff>
--- a/gasPrices.xlsx
+++ b/gasPrices.xlsx
@@ -435,10 +435,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:C37"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2015,9 +2015,639 @@
         </is>
       </c>
       <c r="B105" t="n">
+        <v>45.85</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>08/11/2023 11</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>44.82</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>08/11/2023 12</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>46.16</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>08/11/2023 13</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>48.49</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>08/11/2023 14</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>51.24</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>08/11/2023 15</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>54.65</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>08/11/2023 16</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>53</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>08/11/2023 17</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>51.2</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>08/11/2023 18</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>49.88</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>08/11/2023 19</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>55.95</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>08/11/2023 20</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>239.28</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>08/11/2023 21</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>592.0700000000001</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>08/11/2023 22</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>582.3</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>08/11/2023 23</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>430.45</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>08/11/2023 24</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>320.9</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>08/12/2023 01</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>491</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>08/12/2023 02</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>341.07</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>08/12/2023 03</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>90.7</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>08/12/2023 04</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
         <v>-1</v>
       </c>
-      <c r="C105" t="inlineStr">
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>08/14/2023 09</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>55.03</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>08/14/2023 10</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>64.2</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>08/14/2023 11</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>77.76000000000001</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>08/14/2023 12</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>218.46</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>08/14/2023 19</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>491.44</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>08/14/2023 20</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>710.03</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>08/14/2023 21</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>559.89</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>08/14/2023 22</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>349.73</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>08/14/2023 23</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>233.76</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>08/14/2023 24</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>173.86</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>08/15/2023 01</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>142.91</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>08/15/2023 02</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>68.98999999999999</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>08/15/2023 03</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>53.17</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>08/15/2023 04</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>49.28</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>08/15/2023 05</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>59.62</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>08/15/2023 06</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>155.44</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>08/15/2023 07</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>273.66</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>08/15/2023 08</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>71.54000000000001</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>08/15/2023 09</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>320.14</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>08/15/2023 10</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>111.68</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>08/15/2023 11</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>101.28</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>08/15/2023 12</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>117.42</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>08/15/2023 13</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>269.41</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>08/15/2023 14</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C147" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>